<commit_message>
add exercise session to calender
</commit_message>
<xml_diff>
--- a/div/lectureplan-V25.xlsx
+++ b/div/lectureplan-V25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit.sharepoint.com/teams/GRP_NHHDepartmentofStatistics/Delte dokumenter/Undervisning/TECH3/TECH3_book/div/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{0E369630-2FEA-4A24-B5E7-9A3EFAC6229A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD87094C-7EA0-427E-9BFB-603C8136B2B0}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{0E369630-2FEA-4A24-B5E7-9A3EFAC6229A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{445795C7-04EA-4DF0-9C81-FE2BC1602BE6}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>23.01: &lt;strong&gt;Collaborative learning session&lt;/strong&gt; in Aud J</t>
   </si>
   <si>
-    <t>30.01: &lt;strong&gt;Practical session&lt;/strong&gt; in Aud J</t>
-  </si>
-  <si>
     <t>06.02: &lt;strong&gt;Case session&lt;/strong&gt; in Aud J</t>
   </si>
   <si>
@@ -159,6 +156,10 @@
   </si>
   <si>
     <t>24.04: &lt;strong&gt;Exam prepartion session?&lt;/strong&gt; in Aud J</t>
+  </si>
+  <si>
+    <t>30.01: &lt;strong&gt;
+Exercise session&lt;/strong&gt; in Aud J</t>
   </si>
 </sst>
 </file>
@@ -194,8 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,10 +217,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,7 +519,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +585,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -595,8 +595,8 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -773,15 +773,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2d60b56-d534-48f8-852c-9346ababfcfc">
@@ -790,6 +781,15 @@
     <TaxCatchAll xmlns="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -994,20 +994,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
     <ds:schemaRef ds:uri="1a38ecde-d8a6-449a-a4de-d3c0367a81fe"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
move M3 practical session
</commit_message>
<xml_diff>
--- a/div/lectureplan-V25.xlsx
+++ b/div/lectureplan-V25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit.sharepoint.com/teams/GRP_NHHDepartmentofStatistics/Delte dokumenter/Undervisning/TECH3/TECH3_book/div/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s15052\OneDrive - Norges Handelshøyskole\Undervisning\TECH3\TECH3_book\div\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{0E369630-2FEA-4A24-B5E7-9A3EFAC6229A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{445795C7-04EA-4DF0-9C81-FE2BC1602BE6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F05747-94EB-4E0D-B4C4-6AF79890BAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>17.02: &lt;strong&gt;Overview lecture&lt;/strong&gt; in Aud C</t>
   </si>
   <si>
-    <t>24.02: No lecture</t>
-  </si>
-  <si>
     <t>03:03: &lt;strong&gt;Overview lecture&lt;/strong&gt; in Aud C</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
   </si>
   <si>
     <t>13.02: &lt;strong&gt;Collaborative learning session&lt;/strong&gt; in Aud J</t>
-  </si>
-  <si>
-    <t>20.02: &lt;strong&gt;Practical session&lt;/strong&gt;  in Aud J.</t>
   </si>
   <si>
     <t>27.02: &lt;strong&gt;Case session&lt;/strong&gt; in Aud J</t>
@@ -160,6 +154,12 @@
   <si>
     <t>30.01: &lt;strong&gt;
 Exercise session&lt;/strong&gt; in Aud J</t>
+  </si>
+  <si>
+    <t>24.02: &lt;strong&gt;Practical session&lt;/strong&gt;  in Aud C.</t>
+  </si>
+  <si>
+    <t>20.02: No lecture.</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,10 +649,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,10 +663,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,10 +677,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,10 +691,10 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,10 +705,10 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -719,10 +719,10 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,10 +733,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,10 +747,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,10 +761,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -784,15 +784,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1B0514731AD424F999ECAD5B293E75C" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="791e2903c2d387dd0f8ffbc61bcfe074">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2d60b56-d534-48f8-852c-9346ababfcfc" xmlns:ns3="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79505928d35f7127a600a22198fcd716" ns2:_="" ns3:_="">
     <xsd:import namespace="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
@@ -993,6 +984,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
   <ds:schemaRefs>
@@ -1005,14 +1005,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F9C8970-FADB-48F2-9990-30149F68A38A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1029,4 +1021,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add oracle session to calender
</commit_message>
<xml_diff>
--- a/div/lectureplan-V25.xlsx
+++ b/div/lectureplan-V25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s15052\OneDrive - Norges Handelshøyskole\Undervisning\TECH3\TECH3_book\div\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit.sharepoint.com/teams/GRP_NHHDepartmentofStatistics/Delte dokumenter/Undervisning/TECH3/TECH3_book/div/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F05747-94EB-4E0D-B4C4-6AF79890BAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{70F05747-94EB-4E0D-B4C4-6AF79890BAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAA82237-C834-4FCC-9A97-58A529BD75DB}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,6 @@
     <t>27.02: &lt;strong&gt;Case session&lt;/strong&gt; in Aud J</t>
   </si>
   <si>
-    <t>06.03: No lecture</t>
-  </si>
-  <si>
     <t>13.03: &lt;strong&gt;Collaborative learning session&lt;/strong&gt;  in Aud J.</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>20.02: No lecture.</t>
+  </si>
+  <si>
+    <t>06.03: &lt;strong&gt;Oracle session&lt;/strong&gt; in Aud J</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +596,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
@@ -666,7 +666,7 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -784,6 +784,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1B0514731AD424F999ECAD5B293E75C" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="791e2903c2d387dd0f8ffbc61bcfe074">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2d60b56-d534-48f8-852c-9346ababfcfc" xmlns:ns3="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79505928d35f7127a600a22198fcd716" ns2:_="" ns3:_="">
     <xsd:import namespace="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
@@ -984,15 +993,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
   <ds:schemaRefs>
@@ -1005,6 +1005,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F9C8970-FADB-48F2-9990-30149F68A38A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1021,12 +1029,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>